<commit_message>
fix double lick in calendar vs down file mẫu
</commit_message>
<xml_diff>
--- a/Upload/Customer - Personal.xlsx
+++ b/Upload/Customer - Personal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phuoc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DIP\CRMVT\CRMViettour\Upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>